<commit_message>
Add updated mapping spreadsheet and set default path for it
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheet2templatePath2.0.xlsx
+++ b/src/main/resources/spreadsheet2templatePath2.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ycao77/bmir-radx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ycao77/bmir-radx/radx-rad-metadata-compiler/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180ED520-9526-7740-B787-CBC24D42D9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22013F06-8F76-8F42-9104-176F646778A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="-25700" windowWidth="27640" windowHeight="19560" xr2:uid="{297628F6-E04B-2149-A12F-46F8E7030659}"/>
+    <workbookView xWindow="5320" yWindow="-25700" windowWidth="27640" windowHeight="21640" xr2:uid="{297628F6-E04B-2149-A12F-46F8E7030659}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
   <si>
     <t>RADx-rad Field Label</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>/SHA256 digest</t>
+  </si>
+  <si>
+    <t>/File Name</t>
   </si>
 </sst>
 </file>
@@ -337,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -362,6 +365,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -700,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C9FA6C8-3052-4F44-924C-F8A85A6A2B10}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -974,12 +980,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>40</v>
+      <c r="B34" s="20" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
git add spreadsheet2templatePath2.0.xlsx and modify the filed generators so it returns specific type
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheet2templatePath2.0.xlsx
+++ b/src/main/resources/spreadsheet2templatePath2.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ycao77/bmir-radx/radx-rad-metadata-compiler/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22013F06-8F76-8F42-9104-176F646778A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5A8FC5-1E69-254F-9312-19586DE0AD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="-25700" windowWidth="27640" windowHeight="21640" xr2:uid="{297628F6-E04B-2149-A12F-46F8E7030659}"/>
+    <workbookView xWindow="1820" yWindow="-25700" windowWidth="31140" windowHeight="21640" xr2:uid="{297628F6-E04B-2149-A12F-46F8E7030659}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C9FA6C8-3052-4F44-924C-F8A85A6A2B10}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -877,11 +877,11 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>40</v>
+      <c r="B21" s="18" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>